<commit_message>
small update to exercise 2 solution guide
</commit_message>
<xml_diff>
--- a/Data/E2.xlsx
+++ b/Data/E2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Log" sheetId="2" r:id="rId1"/>
@@ -764,7 +764,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -853,8 +853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,7 +961,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,7 +1087,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1175,9 +1175,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>